<commit_message>
Added better switch status reporting
</commit_message>
<xml_diff>
--- a/docs/HID Message Data Structures.xlsx
+++ b/docs/HID Message Data Structures.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy-daily\Documents\GitHub\SSS2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F62F04-2FA2-4149-AEA9-2837DB88B2F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D98C5F-9A0E-4F45-8269-4E869676C8E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{8EB730A1-2A75-43B6-8245-2760B3944517}"/>
+    <workbookView xWindow="4710" yWindow="1320" windowWidth="26790" windowHeight="14565" firstSheet="1" activeTab="5" xr2:uid="{8EB730A1-2A75-43B6-8245-2760B3944517}"/>
   </bookViews>
   <sheets>
     <sheet name="HID Frame" sheetId="1" r:id="rId1"/>
     <sheet name="Status Pg 1" sheetId="2" r:id="rId2"/>
     <sheet name="Status Pg 1 Description" sheetId="5" r:id="rId3"/>
     <sheet name="Status Pg 2" sheetId="3" r:id="rId4"/>
-    <sheet name="Status Pg 3" sheetId="4" r:id="rId5"/>
+    <sheet name="DAC Calibration" sheetId="6" r:id="rId5"/>
+    <sheet name="HVAdjOut Calibration" sheetId="7" r:id="rId6"/>
+    <sheet name="Status Pg 3" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="317">
   <si>
     <t>Byte</t>
   </si>
@@ -661,9 +663,6 @@
     <t>LIN TX Count</t>
   </si>
   <si>
-    <t>Serial Sequence Number</t>
-  </si>
-  <si>
     <t>NetStatus</t>
   </si>
   <si>
@@ -974,6 +973,21 @@
   </si>
   <si>
     <t>["Potentiometers"]["Others"]["Pairs"]["I2CPots"]["Pots"]["U37"]["Wiper Position"]</t>
+  </si>
+  <si>
+    <t>Counter</t>
+  </si>
+  <si>
+    <t>DAC Slope</t>
+  </si>
+  <si>
+    <t>Setting</t>
+  </si>
+  <si>
+    <t>Millivolts</t>
+  </si>
+  <si>
+    <t>Voltage</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1070,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1088,15 +1102,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1106,10 +1111,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1125,6 +1142,2060 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>DAC</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Calibration</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10580315707950501"/>
+          <c:y val="0.1300462962962963"/>
+          <c:w val="0.85219685039370074"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.874183946724829E-2"/>
+                  <c:y val="0.37187554680664919"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'DAC Calibration'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'DAC Calibration'!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1233</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>618</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1849</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2467</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3083</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3698</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4314</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4931</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C6BB-45EF-BFC3-4B26C342375C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="512865856"/>
+        <c:axId val="620969872"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="512865856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="620969872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="620969872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="512865856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HVAdjOut Calibration'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Voltage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'HVAdjOut Calibration'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>175</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'HVAdjOut Calibration'!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.94</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.3600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.84</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.36</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-027D-4A8F-882F-1FA06628DB34}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="779495920"/>
+        <c:axId val="620956976"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="779495920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="620956976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="620956976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="779495920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE51AE33-2942-4818-AA90-AEB8812DAC45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>357186</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79A1AB43-206F-42B2-97D0-3F88F0BADD78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1509,23 +3580,23 @@
       <c r="B3" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1597,24 +3668,24 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1686,24 +3757,24 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1775,26 +3846,26 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="Q12" s="11"/>
+      <c r="Q12" s="15"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -1912,7 +3983,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F12" sqref="F12:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,125 +3994,125 @@
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="12">
         <v>0</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="12">
         <f>B2+1</f>
         <v>1</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="12">
         <f t="shared" ref="D2:Q2" si="0">C2+1</f>
         <v>2</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="12">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2" s="12">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="L2" s="15">
+      <c r="L2" s="12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M2" s="15">
+      <c r="M2" s="12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="N2" s="15">
+      <c r="N2" s="12">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O2" s="15">
+      <c r="O2" s="12">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="P2" s="15">
+      <c r="P2" s="12">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="Q2" s="15">
+      <c r="Q2" s="12">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="N3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="P3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="Q3" s="13" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2068,105 +4139,105 @@
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="12">
         <f>B2+16</f>
         <v>16</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <f>B5+1</f>
         <v>17</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <f t="shared" ref="D5:Q5" si="1">C5+1</f>
         <v>18</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="12">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="12">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="12">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="12">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="12">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="12">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="12">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="12">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="12">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="12">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="O5" s="15">
+      <c r="O5" s="12">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="P5" s="15">
+      <c r="P5" s="12">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="Q5" s="15">
+      <c r="Q5" s="12">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17" t="s">
+      <c r="D6" s="16"/>
+      <c r="E6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17" t="s">
+      <c r="H6" s="16"/>
+      <c r="I6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17" t="s">
+      <c r="J6" s="16"/>
+      <c r="K6" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17" t="s">
+      <c r="L6" s="16"/>
+      <c r="M6" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17" t="s">
+      <c r="N6" s="16"/>
+      <c r="O6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="16" t="s">
+      <c r="P6" s="16"/>
+      <c r="Q6" s="13" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2193,105 +4264,105 @@
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="12">
         <f>B5+16</f>
         <v>32</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <f>B8+1</f>
         <v>33</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <f t="shared" ref="D8:Q8" si="2">C8+1</f>
         <v>34</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="12">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="12">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="12">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="12">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="12">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="12">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="12">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="12">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="12">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="12">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="O8" s="15">
+      <c r="O8" s="12">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="P8" s="15">
+      <c r="P8" s="12">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="Q8" s="15">
+      <c r="Q8" s="12">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17" t="s">
+      <c r="D9" s="16"/>
+      <c r="E9" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17" t="s">
+      <c r="F9" s="16"/>
+      <c r="G9" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17" t="s">
+      <c r="H9" s="16"/>
+      <c r="I9" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17" t="s">
+      <c r="J9" s="16"/>
+      <c r="K9" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17" t="s">
+      <c r="L9" s="16"/>
+      <c r="M9" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17" t="s">
+      <c r="N9" s="16"/>
+      <c r="O9" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="16" t="s">
+      <c r="P9" s="16"/>
+      <c r="Q9" s="13" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2318,114 +4389,125 @@
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="12">
         <f>B8+16</f>
         <v>48</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="12">
         <f>B11+1</f>
         <v>49</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <f t="shared" ref="D11:Q11" si="3">C11+1</f>
         <v>50</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="12">
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="12">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="12">
         <f t="shared" si="3"/>
         <v>53</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="12">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="12">
         <f t="shared" si="3"/>
         <v>55</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="12">
         <f t="shared" si="3"/>
         <v>56</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="12">
         <f t="shared" si="3"/>
         <v>57</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="12">
         <f t="shared" si="3"/>
         <v>58</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="12">
         <f t="shared" si="3"/>
         <v>59</v>
       </c>
-      <c r="N11" s="15">
+      <c r="N11" s="12">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="O11" s="15">
+      <c r="O11" s="12">
         <f t="shared" si="3"/>
         <v>61</v>
       </c>
-      <c r="P11" s="15">
+      <c r="P11" s="12">
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
-      <c r="Q11" s="15">
+      <c r="Q11" s="12">
         <f t="shared" si="3"/>
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17" t="s">
+      <c r="G12" s="16"/>
+      <c r="H12" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17" t="s">
+      <c r="I12" s="16"/>
+      <c r="J12" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17" t="s">
+      <c r="K12" s="16"/>
+      <c r="L12" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="M12" s="17"/>
-      <c r="N12" s="16" t="s">
+      <c r="M12" s="16"/>
+      <c r="N12" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="O12" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="P12" s="17" t="s">
+      <c r="O12" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="P12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="Q12" s="17"/>
+      <c r="Q12" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="L12:M12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="M9:N9"/>
@@ -2434,17 +4516,6 @@
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="K9:L9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2456,7 +4527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B0F807-5317-404D-A0AA-AC8872219226}">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
@@ -2474,7 +4545,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2485,19 +4556,19 @@
         <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2844,7 +4915,7 @@
         <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D27" t="s">
         <v>91</v>
@@ -2861,7 +4932,7 @@
         <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D28" t="s">
         <v>92</v>
@@ -2878,7 +4949,7 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D29" t="s">
         <v>95</v>
@@ -2895,7 +4966,7 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D30" t="s">
         <v>96</v>
@@ -2912,7 +4983,7 @@
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D31" t="s">
         <v>97</v>
@@ -2929,7 +5000,7 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D32" t="s">
         <v>98</v>
@@ -2946,7 +5017,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D33" t="s">
         <v>99</v>
@@ -2963,7 +5034,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D34" t="s">
         <v>100</v>
@@ -2983,7 +5054,7 @@
         <v>74</v>
       </c>
       <c r="E35" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F35" t="s">
         <v>108</v>
@@ -3000,7 +5071,7 @@
         <v>74</v>
       </c>
       <c r="E36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F36" t="s">
         <v>112</v>
@@ -3017,7 +5088,7 @@
         <v>74</v>
       </c>
       <c r="E37" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F37" t="s">
         <v>113</v>
@@ -3034,7 +5105,7 @@
         <v>74</v>
       </c>
       <c r="E38" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F38" t="s">
         <v>114</v>
@@ -3048,19 +5119,19 @@
         <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D39" t="s">
         <v>95</v>
       </c>
       <c r="E39" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F39" t="s">
         <v>115</v>
       </c>
       <c r="G39" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3071,19 +5142,19 @@
         <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D40" t="s">
         <v>96</v>
       </c>
       <c r="E40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F40" t="s">
         <v>116</v>
       </c>
       <c r="G40" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3094,19 +5165,19 @@
         <v>34</v>
       </c>
       <c r="C41" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D41" t="s">
         <v>99</v>
       </c>
       <c r="E41" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G41" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3117,19 +5188,19 @@
         <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D42" t="s">
         <v>100</v>
       </c>
       <c r="E42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F42" t="s">
         <v>133</v>
       </c>
       <c r="G42" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3140,19 +5211,19 @@
         <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D43" t="s">
         <v>91</v>
       </c>
       <c r="E43" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F43" t="s">
         <v>135</v>
       </c>
       <c r="G43" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3163,19 +5234,19 @@
         <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D44" t="s">
         <v>92</v>
       </c>
       <c r="E44" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F44" t="s">
         <v>136</v>
       </c>
       <c r="G44" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3186,19 +5257,19 @@
         <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D45" t="s">
         <v>95</v>
       </c>
       <c r="E45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F45" t="s">
         <v>137</v>
       </c>
       <c r="G45" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3209,19 +5280,19 @@
         <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D46" t="s">
         <v>96</v>
       </c>
       <c r="E46" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F46" t="s">
         <v>138</v>
       </c>
       <c r="G46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3232,19 +5303,19 @@
         <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D47" t="s">
         <v>91</v>
       </c>
       <c r="E47" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F47" t="s">
         <v>139</v>
       </c>
       <c r="G47" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3255,19 +5326,19 @@
         <v>60</v>
       </c>
       <c r="C48" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D48" t="s">
         <v>92</v>
       </c>
       <c r="E48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F48" t="s">
         <v>140</v>
       </c>
       <c r="G48" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3278,19 +5349,19 @@
         <v>60</v>
       </c>
       <c r="C49" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D49" t="s">
         <v>95</v>
       </c>
       <c r="E49" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F49" t="s">
         <v>141</v>
       </c>
       <c r="G49" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3301,19 +5372,19 @@
         <v>60</v>
       </c>
       <c r="C50" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D50" t="s">
         <v>96</v>
       </c>
       <c r="E50" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F50" t="s">
         <v>142</v>
       </c>
       <c r="G50" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3324,19 +5395,19 @@
         <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D51" t="s">
         <v>55</v>
       </c>
       <c r="E51" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F51" t="s">
         <v>143</v>
       </c>
       <c r="G51" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3347,19 +5418,19 @@
         <v>60</v>
       </c>
       <c r="C52" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D52" t="s">
         <v>100</v>
       </c>
       <c r="E52" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F52" t="s">
         <v>144</v>
       </c>
       <c r="G52" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3370,19 +5441,19 @@
         <v>47</v>
       </c>
       <c r="C53" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D53" t="s">
         <v>97</v>
       </c>
       <c r="E53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F53" t="s">
         <v>145</v>
       </c>
       <c r="G53" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3393,19 +5464,19 @@
         <v>47</v>
       </c>
       <c r="C54" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D54" t="s">
         <v>98</v>
       </c>
       <c r="E54" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F54" t="s">
         <v>146</v>
       </c>
       <c r="G54" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3416,19 +5487,19 @@
         <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D55" t="s">
         <v>99</v>
       </c>
       <c r="E55" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F55" t="s">
         <v>147</v>
       </c>
       <c r="G55" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -3439,19 +5510,19 @@
         <v>47</v>
       </c>
       <c r="C56" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D56" t="s">
         <v>100</v>
       </c>
       <c r="E56" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F56" t="s">
         <v>148</v>
       </c>
       <c r="G56" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3462,19 +5533,19 @@
         <v>34</v>
       </c>
       <c r="C57" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D57" t="s">
         <v>91</v>
       </c>
       <c r="E57" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F57" t="s">
         <v>149</v>
       </c>
       <c r="G57" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3485,19 +5556,19 @@
         <v>34</v>
       </c>
       <c r="C58" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D58" t="s">
         <v>92</v>
       </c>
       <c r="E58" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F58" t="s">
         <v>150</v>
       </c>
       <c r="G58" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3508,19 +5579,19 @@
         <v>34</v>
       </c>
       <c r="C59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D59" t="s">
         <v>97</v>
       </c>
       <c r="E59" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F59" t="s">
         <v>151</v>
       </c>
-      <c r="G59" s="18" t="s">
-        <v>302</v>
+      <c r="G59" s="14" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3531,19 +5602,19 @@
         <v>34</v>
       </c>
       <c r="C60" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D60" t="s">
         <v>98</v>
       </c>
       <c r="E60" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F60" t="s">
         <v>152</v>
       </c>
       <c r="G60" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3554,19 +5625,19 @@
         <v>49</v>
       </c>
       <c r="C61" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D61" t="s">
         <v>55</v>
       </c>
       <c r="E61" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F61" t="s">
         <v>153</v>
       </c>
       <c r="G61" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3577,19 +5648,19 @@
         <v>50</v>
       </c>
       <c r="C62" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D62" t="s">
         <v>55</v>
       </c>
       <c r="E62" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F62" t="s">
         <v>154</v>
       </c>
       <c r="G62" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3600,19 +5671,19 @@
         <v>51</v>
       </c>
       <c r="C63" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D63" t="s">
         <v>55</v>
       </c>
       <c r="E63" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F63" t="s">
         <v>155</v>
       </c>
       <c r="G63" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3626,7 +5697,7 @@
         <v>74</v>
       </c>
       <c r="E64" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F64" t="s">
         <v>162</v>
@@ -3643,7 +5714,7 @@
         <v>74</v>
       </c>
       <c r="E65" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F65" t="s">
         <v>161</v>
@@ -3660,7 +5731,7 @@
         <v>74</v>
       </c>
       <c r="E66" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F66" t="s">
         <v>167</v>
@@ -3677,13 +5748,13 @@
         <v>74</v>
       </c>
       <c r="E67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F67" t="s">
         <v>160</v>
       </c>
       <c r="G67" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3694,19 +5765,19 @@
         <v>61</v>
       </c>
       <c r="C68" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D68" t="s">
         <v>96</v>
       </c>
       <c r="E68" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F68" t="s">
         <v>121</v>
       </c>
       <c r="G68" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3745,19 +5816,19 @@
         <v>61</v>
       </c>
       <c r="C71" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D71" t="s">
         <v>99</v>
       </c>
       <c r="E71" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F71" t="s">
         <v>165</v>
       </c>
       <c r="G71" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3768,19 +5839,19 @@
         <v>61</v>
       </c>
       <c r="C72" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D72" t="s">
         <v>100</v>
       </c>
       <c r="E72" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F72" t="s">
         <v>166</v>
       </c>
       <c r="G72" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3791,19 +5862,19 @@
         <v>61</v>
       </c>
       <c r="C73" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D73" t="s">
         <v>98</v>
       </c>
       <c r="E73" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F73" t="s">
         <v>132</v>
       </c>
       <c r="G73" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3814,7 +5885,7 @@
         <v>61</v>
       </c>
       <c r="C74" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D74" t="s">
         <v>91</v>
@@ -3823,7 +5894,7 @@
         <v>119</v>
       </c>
       <c r="G74" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3834,7 +5905,7 @@
         <v>61</v>
       </c>
       <c r="C75" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D75" t="s">
         <v>92</v>
@@ -3843,7 +5914,7 @@
         <v>120</v>
       </c>
       <c r="G75" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -3854,7 +5925,7 @@
         <v>61</v>
       </c>
       <c r="C76" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D76" t="s">
         <v>95</v>
@@ -3863,7 +5934,7 @@
         <v>118</v>
       </c>
       <c r="G76" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -3876,8 +5947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF52B80C-E677-48BE-9EAF-D32B6CF5339A}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4153,11 +6224,11 @@
       <c r="N6" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="O6" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -4252,29 +6323,29 @@
       <c r="B9" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13" t="s">
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13" t="s">
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13" t="s">
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -4369,35 +6440,37 @@
       <c r="B12" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13" t="s">
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13" t="s">
+      <c r="H12" s="17"/>
+      <c r="I12" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13" t="s">
+      <c r="J12" s="17"/>
+      <c r="K12" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="L12" s="13"/>
+      <c r="L12" s="17"/>
       <c r="M12" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="N12" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="O12" s="14"/>
-      <c r="P12" s="12" t="s">
+      <c r="N12" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="P12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="Q12" s="12"/>
+      <c r="Q12" s="18"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -4429,7 +6502,7 @@
         <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4443,7 +6516,7 @@
         <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -4457,7 +6530,7 @@
         <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4471,7 +6544,7 @@
         <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -4485,7 +6558,7 @@
         <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -4499,7 +6572,7 @@
         <v>55</v>
       </c>
       <c r="D22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -4513,7 +6586,7 @@
         <v>55</v>
       </c>
       <c r="D23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -4527,7 +6600,7 @@
         <v>55</v>
       </c>
       <c r="D24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -4541,7 +6614,7 @@
         <v>55</v>
       </c>
       <c r="D25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -4555,7 +6628,7 @@
         <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4569,7 +6642,7 @@
         <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4583,7 +6656,7 @@
         <v>55</v>
       </c>
       <c r="D28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4597,7 +6670,7 @@
         <v>55</v>
       </c>
       <c r="D29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4611,7 +6684,7 @@
         <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4625,7 +6698,7 @@
         <v>55</v>
       </c>
       <c r="D31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -4639,7 +6712,7 @@
         <v>55</v>
       </c>
       <c r="D32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -4653,7 +6726,7 @@
         <v>55</v>
       </c>
       <c r="D33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4667,7 +6740,7 @@
         <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4681,7 +6754,7 @@
         <v>55</v>
       </c>
       <c r="D35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4692,7 +6765,7 @@
         <v>55</v>
       </c>
       <c r="D36" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -4703,7 +6776,7 @@
         <v>92</v>
       </c>
       <c r="D37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -4714,7 +6787,7 @@
         <v>95</v>
       </c>
       <c r="D38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -4725,11 +6798,11 @@
         <v>96</v>
       </c>
       <c r="D39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="K9:N9"/>
     <mergeCell ref="O9:Q9"/>
@@ -4737,7 +6810,6 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="I12:J12"/>
-    <mergeCell ref="N12:O12"/>
     <mergeCell ref="P12:Q12"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="G9:J9"/>
@@ -4749,11 +6821,249 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8082CC5-179A-43FC-9E22-F59AEB659705}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1000</v>
+      </c>
+      <c r="B2">
+        <v>1233</v>
+      </c>
+      <c r="D2">
+        <f>SLOPE(B2:B11,A2:A11)</f>
+        <v>1.2321680586330321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>500</v>
+      </c>
+      <c r="B3">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1500</v>
+      </c>
+      <c r="B4">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2000</v>
+      </c>
+      <c r="B5">
+        <v>2467</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2500</v>
+      </c>
+      <c r="B6">
+        <v>3083</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3000</v>
+      </c>
+      <c r="B7">
+        <v>3698</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>300</v>
+      </c>
+      <c r="B8">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3500</v>
+      </c>
+      <c r="B9">
+        <v>4314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4000</v>
+      </c>
+      <c r="B10">
+        <v>4931</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF26031-8F5A-46B8-82E8-E414FD86169A}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1.94</v>
+      </c>
+      <c r="D2">
+        <f>SLOPE(B2:B12,A2:A12)</f>
+        <v>4.9441804129657395E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2.19</v>
+      </c>
+      <c r="D3">
+        <f>1/D2</f>
+        <v>20.225799151211707</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>75</v>
+      </c>
+      <c r="B8">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <v>6.84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>125</v>
+      </c>
+      <c r="B10">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>150</v>
+      </c>
+      <c r="B11">
+        <v>9.36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>175</v>
+      </c>
+      <c r="B12">
+        <v>10.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A36B7D-DF26-4857-9B9A-8D2F5EA0B6B1}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4852,34 +7162,34 @@
     <row r="3" spans="1:17" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13" t="s">
+      <c r="H3" s="17"/>
+      <c r="I3" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13" t="s">
+      <c r="P3" s="17"/>
+      <c r="Q3" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="5" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -4973,29 +7283,29 @@
     <row r="6" spans="1:17" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="D6" s="17"/>
+      <c r="E6" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="17"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -5088,21 +7398,21 @@
     <row r="9" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -5195,23 +7505,24 @@
     <row r="12" spans="1:17" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="12" t="s">
+      <c r="O12" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="P12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="Q12" s="12"/>
+      <c r="Q12" s="18"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -5343,8 +7654,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="N12:O12"/>
+  <mergeCells count="18">
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="C6:D6"/>
@@ -5360,9 +7673,6 @@
     <mergeCell ref="K9:N9"/>
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="C12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Support for Threads and CAN
</commit_message>
<xml_diff>
--- a/docs/HID Message Data Structures.xlsx
+++ b/docs/HID Message Data Structures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy-daily\Documents\GitHub\SSS2\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\GitHub\SSS2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0495AD4D-A554-43E5-A6BC-00FFEAF48FAB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064ECA2F-51E0-4AA2-AF5E-FB4D0B4C5487}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="345" windowWidth="24750" windowHeight="14535" firstSheet="2" activeTab="8" xr2:uid="{8EB730A1-2A75-43B6-8245-2760B3944517}"/>
+    <workbookView xWindow="28635" yWindow="4635" windowWidth="27210" windowHeight="16560" firstSheet="1" activeTab="8" xr2:uid="{8EB730A1-2A75-43B6-8245-2760B3944517}"/>
   </bookViews>
   <sheets>
     <sheet name="HID Frame" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="DAC Calibration" sheetId="6" r:id="rId6"/>
     <sheet name="HVAdjOut Calibration" sheetId="7" r:id="rId7"/>
     <sheet name="Status Pg 3" sheetId="4" r:id="rId8"/>
-    <sheet name="CAN (2)" sheetId="9" r:id="rId9"/>
+    <sheet name="CAN Thread" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="383">
   <si>
     <t>Byte</t>
   </si>
@@ -668,9 +668,6 @@
     <t>CAN Thread Size</t>
   </si>
   <si>
-    <t>enableSendComponentInfo</t>
-  </si>
-  <si>
     <t>currentKnob</t>
   </si>
   <si>
@@ -1131,6 +1128,66 @@
   </si>
   <si>
     <t>Channel/DLC</t>
+  </si>
+  <si>
+    <t>stream CAN0 (true,false)</t>
+  </si>
+  <si>
+    <t>stream CAN1 (true,false)</t>
+  </si>
+  <si>
+    <t>stream CAN2 (true,false)</t>
+  </si>
+  <si>
+    <t>stream J1708 (true,false)</t>
+  </si>
+  <si>
+    <t>suppressLIN(true/false)</t>
+  </si>
+  <si>
+    <t>enableSendComponentInfo(treu,false)</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>CAN Threads</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>TX Period</t>
+  </si>
+  <si>
+    <t>TX Delay</t>
+  </si>
+  <si>
+    <t>Num_messages</t>
+  </si>
+  <si>
+    <t>Stop After Count</t>
+  </si>
+  <si>
+    <t>sub_index</t>
+  </si>
+  <si>
+    <t>Thread Name</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>DLC</t>
+  </si>
+  <si>
+    <t>Transmit Number</t>
+  </si>
+  <si>
+    <t>Type 0x40</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1276,6 +1333,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1287,6 +1347,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3656,10 +3725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE6F6CB-EB28-47D4-A803-F3EF028A0046}">
-  <dimension ref="A2:Q26"/>
+  <dimension ref="A2:Q27"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3741,23 +3810,23 @@
       <c r="B3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -3829,24 +3898,24 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -3918,24 +3987,24 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -4007,26 +4076,26 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21" t="s">
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="Q12" s="21"/>
+      <c r="Q12" s="22"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -4051,7 +4120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>121</v>
       </c>
@@ -4059,14 +4128,14 @@
         <v>1</v>
       </c>
       <c r="C17" s="2" t="str">
-        <f t="shared" ref="C17:C19" si="4">DEC2BIN(B17,4)</f>
+        <f t="shared" ref="C17:C20" si="4">DEC2BIN(B17,4)</f>
         <v>0001</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>125</v>
       </c>
@@ -4078,51 +4147,77 @@
         <v>0010</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21">
+        <v>4</v>
+      </c>
+      <c r="C19" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>0100</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
         <v>8</v>
       </c>
-      <c r="C19" s="2" t="str">
+      <c r="C20" s="2" t="str">
         <f t="shared" si="4"/>
         <v>1000</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="D23" s="4"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4155,7 +4250,7 @@
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -4370,34 +4465,34 @@
       <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22" t="s">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22" t="s">
+      <c r="F6" s="23"/>
+      <c r="G6" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22" t="s">
+      <c r="H6" s="23"/>
+      <c r="I6" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22" t="s">
+      <c r="J6" s="23"/>
+      <c r="K6" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22" t="s">
+      <c r="L6" s="23"/>
+      <c r="M6" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22" t="s">
+      <c r="N6" s="23"/>
+      <c r="O6" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="P6" s="22"/>
+      <c r="P6" s="23"/>
       <c r="Q6" s="13" t="s">
         <v>35</v>
       </c>
@@ -4495,34 +4590,34 @@
       <c r="B9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22" t="s">
+      <c r="D9" s="23"/>
+      <c r="E9" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22" t="s">
+      <c r="F9" s="23"/>
+      <c r="G9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22" t="s">
+      <c r="H9" s="23"/>
+      <c r="I9" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22" t="s">
+      <c r="J9" s="23"/>
+      <c r="K9" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22" t="s">
+      <c r="L9" s="23"/>
+      <c r="M9" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22" t="s">
+      <c r="N9" s="23"/>
+      <c r="O9" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="P9" s="22"/>
+      <c r="P9" s="23"/>
       <c r="Q9" s="13" t="s">
         <v>132</v>
       </c>
@@ -4633,30 +4728,30 @@
         <v>115</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>346</v>
-      </c>
-      <c r="H12" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="H12" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22" t="s">
+      <c r="I12" s="23"/>
+      <c r="J12" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22" t="s">
+      <c r="K12" s="23"/>
+      <c r="L12" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="M12" s="22"/>
+      <c r="M12" s="23"/>
       <c r="N12" s="13" t="s">
         <v>120</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>306</v>
-      </c>
-      <c r="P12" s="22" t="s">
+        <v>305</v>
+      </c>
+      <c r="P12" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="Q12" s="22"/>
+      <c r="Q12" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -4707,7 +4802,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4718,19 +4813,19 @@
         <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D2" t="s">
         <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F2" t="s">
         <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -5077,7 +5172,7 @@
         <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D27" t="s">
         <v>89</v>
@@ -5094,7 +5189,7 @@
         <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D28" t="s">
         <v>90</v>
@@ -5111,7 +5206,7 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D29" t="s">
         <v>93</v>
@@ -5128,7 +5223,7 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D30" t="s">
         <v>94</v>
@@ -5145,7 +5240,7 @@
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D31" t="s">
         <v>95</v>
@@ -5162,7 +5257,7 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D32" t="s">
         <v>96</v>
@@ -5179,7 +5274,7 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D33" t="s">
         <v>97</v>
@@ -5196,7 +5291,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D34" t="s">
         <v>98</v>
@@ -5213,13 +5308,13 @@
         <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D35" t="s">
         <v>72</v>
       </c>
       <c r="E35" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F35" t="s">
         <v>106</v>
@@ -5233,13 +5328,13 @@
         <v>107</v>
       </c>
       <c r="C36" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D36" t="s">
         <v>72</v>
       </c>
       <c r="E36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F36" t="s">
         <v>110</v>
@@ -5253,13 +5348,13 @@
         <v>108</v>
       </c>
       <c r="C37" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D37" t="s">
         <v>72</v>
       </c>
       <c r="E37" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F37" t="s">
         <v>111</v>
@@ -5273,13 +5368,13 @@
         <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D38" t="s">
         <v>72</v>
       </c>
       <c r="E38" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F38" t="s">
         <v>112</v>
@@ -5293,19 +5388,19 @@
         <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D39" t="s">
         <v>93</v>
       </c>
       <c r="E39" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F39" t="s">
         <v>113</v>
       </c>
       <c r="G39" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -5316,19 +5411,19 @@
         <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D40" t="s">
         <v>94</v>
       </c>
       <c r="E40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F40" t="s">
         <v>114</v>
       </c>
       <c r="G40" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -5339,19 +5434,19 @@
         <v>34</v>
       </c>
       <c r="C41" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D41" t="s">
         <v>97</v>
       </c>
       <c r="E41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F41" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -5362,19 +5457,19 @@
         <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D42" t="s">
         <v>98</v>
       </c>
       <c r="E42" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F42" t="s">
         <v>131</v>
       </c>
       <c r="G42" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -5385,19 +5480,19 @@
         <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D43" t="s">
         <v>89</v>
       </c>
       <c r="E43" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F43" t="s">
         <v>133</v>
       </c>
       <c r="G43" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -5408,19 +5503,19 @@
         <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D44" t="s">
         <v>90</v>
       </c>
       <c r="E44" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F44" t="s">
         <v>134</v>
       </c>
       <c r="G44" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -5431,19 +5526,19 @@
         <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D45" t="s">
         <v>93</v>
       </c>
       <c r="E45" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F45" t="s">
         <v>135</v>
       </c>
       <c r="G45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -5454,19 +5549,19 @@
         <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D46" t="s">
         <v>94</v>
       </c>
       <c r="E46" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F46" t="s">
         <v>136</v>
       </c>
       <c r="G46" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -5477,19 +5572,19 @@
         <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D47" t="s">
         <v>89</v>
       </c>
       <c r="E47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F47" t="s">
         <v>137</v>
       </c>
       <c r="G47" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -5500,19 +5595,19 @@
         <v>60</v>
       </c>
       <c r="C48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D48" t="s">
         <v>90</v>
       </c>
       <c r="E48" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F48" t="s">
         <v>138</v>
       </c>
       <c r="G48" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -5523,19 +5618,19 @@
         <v>60</v>
       </c>
       <c r="C49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D49" t="s">
         <v>93</v>
       </c>
       <c r="E49" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F49" t="s">
         <v>139</v>
       </c>
       <c r="G49" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -5546,19 +5641,19 @@
         <v>60</v>
       </c>
       <c r="C50" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D50" t="s">
         <v>94</v>
       </c>
       <c r="E50" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F50" t="s">
         <v>140</v>
       </c>
       <c r="G50" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -5569,19 +5664,19 @@
         <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D51" t="s">
         <v>53</v>
       </c>
       <c r="E51" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F51" t="s">
         <v>141</v>
       </c>
       <c r="G51" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -5592,19 +5687,19 @@
         <v>60</v>
       </c>
       <c r="C52" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D52" t="s">
         <v>98</v>
       </c>
       <c r="E52" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F52" t="s">
         <v>142</v>
       </c>
       <c r="G52" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -5615,19 +5710,19 @@
         <v>47</v>
       </c>
       <c r="C53" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D53" t="s">
         <v>95</v>
       </c>
       <c r="E53" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F53" t="s">
         <v>143</v>
       </c>
       <c r="G53" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -5638,19 +5733,19 @@
         <v>47</v>
       </c>
       <c r="C54" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D54" t="s">
         <v>96</v>
       </c>
       <c r="E54" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F54" t="s">
         <v>144</v>
       </c>
       <c r="G54" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -5661,19 +5756,19 @@
         <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D55" t="s">
         <v>97</v>
       </c>
       <c r="E55" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F55" t="s">
         <v>145</v>
       </c>
       <c r="G55" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -5684,19 +5779,19 @@
         <v>47</v>
       </c>
       <c r="C56" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D56" t="s">
         <v>98</v>
       </c>
       <c r="E56" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F56" t="s">
         <v>146</v>
       </c>
       <c r="G56" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -5707,19 +5802,19 @@
         <v>34</v>
       </c>
       <c r="C57" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D57" t="s">
         <v>89</v>
       </c>
       <c r="E57" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F57" t="s">
         <v>147</v>
       </c>
       <c r="G57" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -5730,19 +5825,19 @@
         <v>34</v>
       </c>
       <c r="C58" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D58" t="s">
         <v>90</v>
       </c>
       <c r="E58" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F58" t="s">
         <v>148</v>
       </c>
       <c r="G58" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -5753,19 +5848,19 @@
         <v>34</v>
       </c>
       <c r="C59" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D59" t="s">
         <v>95</v>
       </c>
       <c r="E59" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F59" t="s">
         <v>149</v>
       </c>
       <c r="G59" s="14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -5776,19 +5871,19 @@
         <v>34</v>
       </c>
       <c r="C60" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D60" t="s">
         <v>96</v>
       </c>
       <c r="E60" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F60" t="s">
         <v>150</v>
       </c>
       <c r="G60" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -5799,19 +5894,19 @@
         <v>49</v>
       </c>
       <c r="C61" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D61" t="s">
         <v>53</v>
       </c>
       <c r="E61" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F61" t="s">
         <v>151</v>
       </c>
       <c r="G61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -5822,19 +5917,19 @@
         <v>50</v>
       </c>
       <c r="C62" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D62" t="s">
         <v>53</v>
       </c>
       <c r="E62" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F62" t="s">
         <v>152</v>
       </c>
       <c r="G62" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -5845,19 +5940,19 @@
         <v>51</v>
       </c>
       <c r="C63" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D63" t="s">
         <v>53</v>
       </c>
       <c r="E63" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F63" t="s">
         <v>153</v>
       </c>
       <c r="G63" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -5871,7 +5966,7 @@
         <v>72</v>
       </c>
       <c r="E64" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -5882,16 +5977,16 @@
         <v>154</v>
       </c>
       <c r="C65" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D65" t="s">
         <v>72</v>
       </c>
       <c r="E65" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F65" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -5902,13 +5997,13 @@
         <v>155</v>
       </c>
       <c r="C66" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D66" t="s">
         <v>72</v>
       </c>
       <c r="E66" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F66" t="s">
         <v>162</v>
@@ -5922,19 +6017,19 @@
         <v>156</v>
       </c>
       <c r="C67" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D67" t="s">
         <v>72</v>
       </c>
       <c r="E67" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F67" t="s">
         <v>157</v>
       </c>
       <c r="G67" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -5945,19 +6040,19 @@
         <v>52</v>
       </c>
       <c r="C68" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D68" t="s">
         <v>94</v>
       </c>
       <c r="E68" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F68" t="s">
         <v>119</v>
       </c>
       <c r="G68" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -5968,7 +6063,7 @@
         <v>128</v>
       </c>
       <c r="C69" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D69" t="s">
         <v>72</v>
@@ -5985,7 +6080,7 @@
         <v>129</v>
       </c>
       <c r="C70" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D70" t="s">
         <v>72</v>
@@ -6002,19 +6097,19 @@
         <v>52</v>
       </c>
       <c r="C71" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D71" t="s">
         <v>97</v>
       </c>
       <c r="E71" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F71" t="s">
         <v>160</v>
       </c>
       <c r="G71" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -6025,19 +6120,19 @@
         <v>52</v>
       </c>
       <c r="C72" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D72" t="s">
         <v>98</v>
       </c>
       <c r="E72" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F72" t="s">
         <v>161</v>
       </c>
       <c r="G72" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -6048,19 +6143,19 @@
         <v>52</v>
       </c>
       <c r="C73" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D73" t="s">
         <v>96</v>
       </c>
       <c r="E73" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F73" t="s">
         <v>130</v>
       </c>
       <c r="G73" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -6071,7 +6166,7 @@
         <v>52</v>
       </c>
       <c r="C74" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D74" t="s">
         <v>89</v>
@@ -6080,7 +6175,7 @@
         <v>117</v>
       </c>
       <c r="G74" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -6091,7 +6186,7 @@
         <v>52</v>
       </c>
       <c r="C75" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D75" t="s">
         <v>90</v>
@@ -6100,7 +6195,7 @@
         <v>118</v>
       </c>
       <c r="G75" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -6111,7 +6206,7 @@
         <v>52</v>
       </c>
       <c r="C76" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D76" t="s">
         <v>93</v>
@@ -6120,7 +6215,7 @@
         <v>116</v>
       </c>
       <c r="G76" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -6229,36 +6324,36 @@
     <row r="3" spans="1:17" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="19" t="s">
+        <v>347</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>348</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="19" t="s">
+        <v>362</v>
+      </c>
+      <c r="H3" s="24" t="s">
         <v>349</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="19" t="s">
-        <v>363</v>
-      </c>
-      <c r="H3" s="23" t="s">
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24" t="s">
         <v>350</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23" t="s">
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="19" t="s">
         <v>351</v>
       </c>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="19" t="s">
+      <c r="P3" s="19" t="s">
         <v>352</v>
       </c>
-      <c r="P3" s="19" t="s">
+      <c r="Q3" s="19" t="s">
         <v>353</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -6352,39 +6447,39 @@
     <row r="6" spans="1:17" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>355</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="D6" s="19" t="s">
         <v>356</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="F6" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="G6" s="23" t="s">
-        <v>360</v>
-      </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
       <c r="K6" s="19" t="s">
-        <v>363</v>
-      </c>
-      <c r="L6" s="23" t="s">
+        <v>362</v>
+      </c>
+      <c r="L6" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24" t="s">
         <v>350</v>
       </c>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23" t="s">
-        <v>351</v>
-      </c>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
@@ -6477,45 +6572,45 @@
     <row r="9" spans="1:17" ht="45.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="K9" s="24" t="s">
         <v>361</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>354</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="K9" s="23" t="s">
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="19" t="s">
         <v>362</v>
       </c>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="19" t="s">
-        <v>363</v>
-      </c>
-      <c r="P9" s="25" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q9" s="25"/>
+      <c r="P9" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="Q9" s="26"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
@@ -6608,58 +6703,58 @@
     <row r="12" spans="1:17" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>350</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="8" t="s">
+      <c r="H12" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="I12" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="J12" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="K12" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="L12" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="M12" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="N12" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="N12" s="8" t="s">
-        <v>359</v>
-      </c>
       <c r="O12" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="P12" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="P12" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="Q12" s="24"/>
+      <c r="Q12" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O6:Q6"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="P12:Q12"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="L6:N6"/>
     <mergeCell ref="K9:N9"/>
     <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O6:Q6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6667,10 +6762,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF52B80C-E677-48BE-9EAF-D32B6CF5339A}">
-  <dimension ref="A1:Q44"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12:Q12"/>
+      <selection activeCell="G9" sqref="G9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6766,7 +6861,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="5" t="s">
         <v>163</v>
@@ -6946,11 +7041,11 @@
       <c r="N6" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="O6" s="23" t="s">
+      <c r="O6" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -7045,29 +7140,29 @@
       <c r="B9" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23" t="s">
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23" t="s">
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23" t="s">
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -7162,24 +7257,24 @@
       <c r="B12" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23" t="s">
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23" t="s">
+      <c r="H12" s="24"/>
+      <c r="I12" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23" t="s">
+      <c r="J12" s="24"/>
+      <c r="K12" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="L12" s="23"/>
+      <c r="L12" s="24"/>
       <c r="M12" s="2" t="s">
         <v>203</v>
       </c>
@@ -7187,12 +7282,12 @@
         <v>115</v>
       </c>
       <c r="O12" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="P12" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="P12" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="Q12" s="24"/>
+      <c r="Q12" s="25"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -7213,7 +7308,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>51</v>
       </c>
@@ -7224,13 +7319,13 @@
         <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>211</v>
-      </c>
-      <c r="L17" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="N17" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>52</v>
       </c>
@@ -7241,13 +7336,13 @@
         <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>212</v>
-      </c>
-      <c r="L18" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="N18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>53</v>
       </c>
@@ -7258,16 +7353,16 @@
         <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>213</v>
-      </c>
-      <c r="L19" t="s">
+        <v>212</v>
+      </c>
+      <c r="N19" t="s">
+        <v>310</v>
+      </c>
+      <c r="O19" t="s">
         <v>311</v>
       </c>
-      <c r="M19" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>54</v>
       </c>
@@ -7278,16 +7373,16 @@
         <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>214</v>
-      </c>
-      <c r="L20">
+        <v>213</v>
+      </c>
+      <c r="N20">
         <v>0</v>
       </c>
-      <c r="M20" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O20" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>55</v>
       </c>
@@ -7298,16 +7393,16 @@
         <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>215</v>
-      </c>
-      <c r="L21">
+        <v>214</v>
+      </c>
+      <c r="N21">
         <v>1</v>
       </c>
-      <c r="M21" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O21" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>56</v>
       </c>
@@ -7318,16 +7413,16 @@
         <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>216</v>
-      </c>
-      <c r="L22">
+        <v>215</v>
+      </c>
+      <c r="N22">
         <v>2</v>
       </c>
-      <c r="M22" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O22" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>57</v>
       </c>
@@ -7338,16 +7433,16 @@
         <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>217</v>
-      </c>
-      <c r="L23">
+        <v>216</v>
+      </c>
+      <c r="N23">
         <v>3</v>
       </c>
-      <c r="M23" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O23" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>58</v>
       </c>
@@ -7358,16 +7453,16 @@
         <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>218</v>
-      </c>
-      <c r="L24">
+        <v>217</v>
+      </c>
+      <c r="N24">
         <v>4</v>
       </c>
-      <c r="M24" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O24" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>59</v>
       </c>
@@ -7378,16 +7473,22 @@
         <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>219</v>
-      </c>
-      <c r="L25">
+        <v>218</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="N25">
         <v>5</v>
       </c>
-      <c r="M25" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O25" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>60</v>
       </c>
@@ -7398,16 +7499,25 @@
         <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>220</v>
-      </c>
-      <c r="L26">
+        <v>219</v>
+      </c>
+      <c r="I26" t="s">
+        <v>70</v>
+      </c>
+      <c r="J26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K26" t="s">
+        <v>369</v>
+      </c>
+      <c r="N26">
         <v>6</v>
       </c>
-      <c r="M26" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O26" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>61</v>
       </c>
@@ -7418,25 +7528,25 @@
         <v>53</v>
       </c>
       <c r="D27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I27" s="1">
         <v>59</v>
       </c>
       <c r="J27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K27" t="s">
-        <v>204</v>
-      </c>
-      <c r="L27">
+        <v>363</v>
+      </c>
+      <c r="N27">
         <v>7</v>
       </c>
-      <c r="M27" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O27" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>62</v>
       </c>
@@ -7447,25 +7557,25 @@
         <v>53</v>
       </c>
       <c r="D28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I28" s="1">
         <v>59</v>
       </c>
       <c r="J28" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K28" t="s">
-        <v>205</v>
-      </c>
-      <c r="L28">
+        <v>364</v>
+      </c>
+      <c r="N28">
         <v>8</v>
       </c>
-      <c r="M28" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O28" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>63</v>
       </c>
@@ -7476,25 +7586,25 @@
         <v>53</v>
       </c>
       <c r="D29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I29" s="1">
         <v>59</v>
       </c>
       <c r="J29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K29" t="s">
-        <v>209</v>
-      </c>
-      <c r="L29">
+        <v>365</v>
+      </c>
+      <c r="N29">
         <v>9</v>
       </c>
-      <c r="M29" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O29" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>64</v>
       </c>
@@ -7505,17 +7615,25 @@
         <v>53</v>
       </c>
       <c r="D30" t="s">
-        <v>224</v>
-      </c>
-      <c r="J30" s="1"/>
-      <c r="L30">
+        <v>223</v>
+      </c>
+      <c r="I30" s="1">
+        <v>59</v>
+      </c>
+      <c r="J30" t="s">
+        <v>94</v>
+      </c>
+      <c r="K30" t="s">
+        <v>366</v>
+      </c>
+      <c r="N30">
         <v>10</v>
       </c>
-      <c r="M30" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O30" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>65</v>
       </c>
@@ -7526,16 +7644,25 @@
         <v>53</v>
       </c>
       <c r="D31" t="s">
-        <v>225</v>
-      </c>
-      <c r="L31">
+        <v>224</v>
+      </c>
+      <c r="I31" s="1">
+        <v>59</v>
+      </c>
+      <c r="J31" t="s">
+        <v>95</v>
+      </c>
+      <c r="K31" t="s">
+        <v>204</v>
+      </c>
+      <c r="N31">
         <v>11</v>
       </c>
-      <c r="M31" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O31" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>66</v>
       </c>
@@ -7546,16 +7673,25 @@
         <v>53</v>
       </c>
       <c r="D32" t="s">
-        <v>226</v>
-      </c>
-      <c r="L32">
+        <v>225</v>
+      </c>
+      <c r="I32" s="1">
+        <v>59</v>
+      </c>
+      <c r="J32" t="s">
+        <v>96</v>
+      </c>
+      <c r="K32" t="s">
+        <v>205</v>
+      </c>
+      <c r="N32">
         <v>12</v>
       </c>
-      <c r="M32" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O32" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>78</v>
       </c>
@@ -7566,16 +7702,25 @@
         <v>53</v>
       </c>
       <c r="D33" t="s">
-        <v>227</v>
-      </c>
-      <c r="L33">
+        <v>226</v>
+      </c>
+      <c r="I33" s="1">
+        <v>59</v>
+      </c>
+      <c r="J33" t="s">
+        <v>97</v>
+      </c>
+      <c r="K33" t="s">
+        <v>368</v>
+      </c>
+      <c r="N33">
         <v>13</v>
       </c>
-      <c r="M33" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O33" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>79</v>
       </c>
@@ -7586,16 +7731,25 @@
         <v>53</v>
       </c>
       <c r="D34" t="s">
-        <v>228</v>
-      </c>
-      <c r="L34">
+        <v>227</v>
+      </c>
+      <c r="I34" s="1">
+        <v>59</v>
+      </c>
+      <c r="J34" t="s">
+        <v>98</v>
+      </c>
+      <c r="K34" t="s">
+        <v>367</v>
+      </c>
+      <c r="N34">
         <v>14</v>
       </c>
-      <c r="M34" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O34" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>80</v>
       </c>
@@ -7606,16 +7760,16 @@
         <v>53</v>
       </c>
       <c r="D35" t="s">
-        <v>229</v>
-      </c>
-      <c r="L35">
+        <v>228</v>
+      </c>
+      <c r="N35">
         <v>15</v>
       </c>
-      <c r="M35" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O35" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>20</v>
       </c>
@@ -7623,10 +7777,10 @@
         <v>53</v>
       </c>
       <c r="D36" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>21</v>
       </c>
@@ -7637,7 +7791,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>22</v>
       </c>
@@ -7645,10 +7799,10 @@
         <v>53</v>
       </c>
       <c r="D38" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>23</v>
       </c>
@@ -7656,10 +7810,10 @@
         <v>53</v>
       </c>
       <c r="D39" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>24</v>
       </c>
@@ -7667,10 +7821,10 @@
         <v>53</v>
       </c>
       <c r="D40" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <v>25</v>
       </c>
@@ -7678,10 +7832,10 @@
         <v>53</v>
       </c>
       <c r="D41" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <v>26</v>
       </c>
@@ -7689,10 +7843,10 @@
         <v>53</v>
       </c>
       <c r="D42" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
         <v>27</v>
       </c>
@@ -7700,10 +7854,10 @@
         <v>53</v>
       </c>
       <c r="D43" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
         <v>28</v>
       </c>
@@ -7711,11 +7865,17 @@
         <v>53</v>
       </c>
       <c r="D44" t="s">
-        <v>337</v>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="I25:L25"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="K9:N9"/>
     <mergeCell ref="O9:Q9"/>
@@ -7748,13 +7908,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" t="s">
         <v>308</v>
       </c>
-      <c r="B1" t="s">
-        <v>309</v>
-      </c>
       <c r="D1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7863,10 +8023,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -8077,32 +8237,32 @@
       <c r="B3" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23" t="s">
+      <c r="H3" s="24"/>
+      <c r="I3" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23" t="s">
+      <c r="P3" s="24"/>
+      <c r="Q3" s="5" t="s">
         <v>232</v>
-      </c>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="5" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -8196,29 +8356,29 @@
     <row r="6" spans="1:17" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="D6" s="24"/>
+      <c r="E6" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23" t="s">
+      <c r="F6" s="24"/>
+      <c r="G6" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="H6" s="23"/>
+      <c r="H6" s="24"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -8311,21 +8471,21 @@
     <row r="9" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -8418,24 +8578,24 @@
     <row r="12" spans="1:17" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
       <c r="M12" s="2"/>
       <c r="O12" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="P12" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="P12" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="Q12" s="24"/>
+      <c r="Q12" s="25"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -8568,6 +8728,10 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="P12:Q12"/>
@@ -8582,10 +8746,6 @@
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -8597,7 +8757,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9:M9"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8689,46 +8849,39 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="19" t="s">
-        <v>348</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>351</v>
-      </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="19" t="s">
-        <v>363</v>
-      </c>
+        <v>382</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>371</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="15" t="s">
+        <v>376</v>
+      </c>
+      <c r="G3" s="15"/>
       <c r="H3" s="19" t="s">
-        <v>352</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>353</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>354</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>355</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>356</v>
-      </c>
-      <c r="M3" s="19" t="s">
-        <v>357</v>
-      </c>
-      <c r="N3" s="19" t="s">
-        <v>358</v>
-      </c>
-      <c r="O3" s="19" t="s">
-        <v>359</v>
-      </c>
-      <c r="P3" s="19" t="s">
-        <v>361</v>
+        <v>380</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>372</v>
+      </c>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24" t="s">
+        <v>373</v>
+      </c>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="19" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -8819,47 +8972,43 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="37.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
-      <c r="B6" s="23" t="s">
-        <v>361</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="19" t="s">
-        <v>363</v>
-      </c>
-      <c r="E6" s="19" t="s">
+      <c r="B6" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24" t="s">
+        <v>350</v>
+      </c>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="K6" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="L6" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="M6" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="N6" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="O6" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="P6" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="Q6" s="8" t="s">
         <v>358</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>359</v>
-      </c>
-      <c r="M6" s="23" t="s">
-        <v>351</v>
-      </c>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="19" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -8952,48 +9101,28 @@
     </row>
     <row r="9" spans="1:17" ht="45.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
-      <c r="B9" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>354</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>361</v>
-      </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="19" t="s">
-        <v>363</v>
-      </c>
-      <c r="O9" s="19" t="s">
-        <v>352</v>
-      </c>
-      <c r="P9" s="19" t="s">
-        <v>353</v>
-      </c>
-      <c r="Q9" s="19" t="s">
-        <v>354</v>
-      </c>
+      <c r="B9" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>381</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="24" t="s">
+        <v>377</v>
+      </c>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
@@ -9083,62 +9212,42 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="38.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
-      <c r="B12" s="19" t="s">
-        <v>355</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>356</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>357</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>358</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>359</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>354</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="B12" s="24" t="s">
+        <v>377</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
       <c r="O12" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="P12" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="P12" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="Q12" s="24"/>
+      <c r="Q12" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="B6:E6"/>
     <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="M6:P6"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="B12:N12"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="G9:Q9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>